<commit_message>
Add test find duplicates in sector
</commit_message>
<xml_diff>
--- a/Sudoku_Grid.xlsx
+++ b/Sudoku_Grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\soe-mobile-sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C650A5E-AF18-49CC-B182-518E697CD831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91056B73-70F4-46F9-AB60-F877D0592402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="4" xr2:uid="{8CBA904F-269B-4B80-8211-F0CFD0911C38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{8CBA904F-269B-4B80-8211-F0CFD0911C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6 (2)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="342">
   <si>
     <t xml:space="preserve"> Field01 = sudokuStringArray[0];</t>
   </si>
@@ -1052,6 +1054,18 @@
   </si>
   <si>
     <t>FieldColor81</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>",</t>
+  </si>
+  <si>
+    <t>"}</t>
+  </si>
+  <si>
+    <t>{"</t>
   </si>
 </sst>
 </file>
@@ -3450,7 +3464,7 @@
         <v>6</v>
       </c>
       <c r="H73" s="12" t="str">
-        <f t="shared" ref="H73:H136" si="1">C73&amp;D73&amp;E73&amp;F73&amp;G73</f>
+        <f t="shared" ref="H73:H87" si="1">C73&amp;D73&amp;E73&amp;F73&amp;G73</f>
         <v>Field67=sudokuStringArray[66];</v>
       </c>
     </row>
@@ -5862,7 +5876,7 @@
         <v>89</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" ref="J71:J134" si="1">D71&amp;E71&amp;F71&amp;G71&amp;H71</f>
+        <f t="shared" ref="J71:J85" si="1">D71&amp;E71&amp;F71&amp;G71&amp;H71</f>
         <v>stringArrayFromFields[66]=Field67;</v>
       </c>
     </row>
@@ -7110,7 +7124,7 @@
         <v>253</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" ref="I27:I90" si="1">C27&amp;D27&amp;E27&amp;F27&amp;G27</f>
+        <f t="shared" ref="I27:I86" si="1">C27&amp;D27&amp;E27&amp;F27&amp;G27</f>
         <v>IsEnabled22=String.IsNullOrEmpty(sudokuStringArray[21])? "true":"false";</v>
       </c>
     </row>
@@ -8407,7 +8421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE7FA67-3B85-4D66-8F07-D6BFFD057CF0}">
   <dimension ref="C3:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H85" sqref="H5:H85"/>
     </sheetView>
   </sheetViews>
@@ -9607,7 +9621,7 @@
         <v>256</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" ref="H70:H111" si="1">C70&amp;D70&amp;E70&amp;F70</f>
+        <f t="shared" ref="H70:H85" si="1">C70&amp;D70&amp;E70&amp;F70</f>
         <v>FieldColor66 = Enum.GetName(typeof(FieldColor), fieldColorArray[65]);</v>
       </c>
     </row>
@@ -9990,4 +10004,2484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96F4CB0-1FB2-4D82-ACB0-0C881D5B76C8}">
+  <dimension ref="G7:K88"/>
+  <sheetViews>
+    <sheetView topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="139.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f>J8&amp;J9&amp;J10&amp;J11&amp;J12&amp;J13&amp;J14&amp;J15&amp;J16&amp;J17&amp;J18&amp;J19&amp;J20&amp;J21&amp;J22&amp;J23&amp;J24&amp;J25&amp;J26&amp;J27&amp;J28&amp;J29&amp;J30&amp;J31&amp;J32&amp;J33&amp;J34&amp;J35&amp;J36&amp;J37&amp;J38&amp;J39&amp;J40&amp;J41&amp;J42&amp;J43&amp;J44&amp;J45&amp;J46&amp;J47&amp;J48&amp;J49&amp;J50&amp;J51&amp;J52&amp;J53&amp;J54&amp;J55&amp;J56&amp;J57&amp;J58&amp;J59&amp;J60&amp;J61&amp;J62&amp;J63&amp;J64&amp;J65&amp;J66&amp;J67&amp;J68&amp;J69&amp;J70&amp;J71&amp;J72&amp;J73&amp;J74&amp;J75&amp;J76&amp;J77&amp;J78&amp;J79&amp;J80&amp;J81&amp;J82&amp;J83&amp;J84&amp;J85&amp;J86&amp;J87&amp;J88</f>
+        <v>"1","2","3","4","5","6","7","8","9","10","11","12","13","14","15","16","17","18","19","20","21","22","23","24","25","26","27","28","29","30","31","32","33","34","35","36","37","38","39","40","41","42","43","44","45","46","47","48","49","50","51","52","53","54","55","56","57","58","59","60","61","62","63","64","65","66","67","68","69","70","71","72","73","74","75","76","77","78","79","80","81",</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>338</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>339</v>
+      </c>
+      <c r="J8" t="str">
+        <f>G8&amp;H8&amp;I8</f>
+        <v>"1",</v>
+      </c>
+    </row>
+    <row r="9" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>339</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9:J39" si="0">G9&amp;H9&amp;I9</f>
+        <v>"2",</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>338</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>339</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>"3",</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>338</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>339</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>"4",</v>
+      </c>
+    </row>
+    <row r="12" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>339</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>"5",</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>338</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>339</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>"6",</v>
+      </c>
+    </row>
+    <row r="14" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>338</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>339</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>"7",</v>
+      </c>
+    </row>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>338</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>339</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>"8",</v>
+      </c>
+    </row>
+    <row r="16" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>339</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>"9",</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>338</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>339</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>"10",</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>338</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>339</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>"11",</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>338</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
+        <v>339</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>"12",</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>338</v>
+      </c>
+      <c r="H20">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>339</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>"13",</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>338</v>
+      </c>
+      <c r="H21">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>339</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>"14",</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>338</v>
+      </c>
+      <c r="H22">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>339</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>"15",</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>339</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>"16",</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>338</v>
+      </c>
+      <c r="H24">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>339</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>"17",</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>338</v>
+      </c>
+      <c r="H25">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>339</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>"18",</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>338</v>
+      </c>
+      <c r="H26">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>339</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>"19",</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>338</v>
+      </c>
+      <c r="H27">
+        <v>20</v>
+      </c>
+      <c r="I27" t="s">
+        <v>339</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>"20",</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>338</v>
+      </c>
+      <c r="H28">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>339</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>"21",</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>338</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29" t="s">
+        <v>339</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>"22",</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>338</v>
+      </c>
+      <c r="H30">
+        <v>23</v>
+      </c>
+      <c r="I30" t="s">
+        <v>339</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>"23",</v>
+      </c>
+    </row>
+    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>338</v>
+      </c>
+      <c r="H31">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>339</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>"24",</v>
+      </c>
+    </row>
+    <row r="32" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>338</v>
+      </c>
+      <c r="H32">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>339</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>"25",</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>338</v>
+      </c>
+      <c r="H33">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
+        <v>339</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>"26",</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>338</v>
+      </c>
+      <c r="H34">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
+        <v>339</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>"27",</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>338</v>
+      </c>
+      <c r="H35">
+        <v>28</v>
+      </c>
+      <c r="I35" t="s">
+        <v>339</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>"28",</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>338</v>
+      </c>
+      <c r="H36">
+        <v>29</v>
+      </c>
+      <c r="I36" t="s">
+        <v>339</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>"29",</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>338</v>
+      </c>
+      <c r="H37">
+        <v>30</v>
+      </c>
+      <c r="I37" t="s">
+        <v>339</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>"30",</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>338</v>
+      </c>
+      <c r="H38">
+        <v>31</v>
+      </c>
+      <c r="I38" t="s">
+        <v>339</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>"31",</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>338</v>
+      </c>
+      <c r="H39">
+        <v>32</v>
+      </c>
+      <c r="I39" t="s">
+        <v>339</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>"32",</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>338</v>
+      </c>
+      <c r="H40">
+        <v>33</v>
+      </c>
+      <c r="I40" t="s">
+        <v>339</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" ref="J40:J46" si="1">G40&amp;H40&amp;I40</f>
+        <v>"33",</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>338</v>
+      </c>
+      <c r="H41">
+        <v>34</v>
+      </c>
+      <c r="I41" t="s">
+        <v>339</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v>"34",</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>338</v>
+      </c>
+      <c r="H42">
+        <v>35</v>
+      </c>
+      <c r="I42" t="s">
+        <v>339</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="1"/>
+        <v>"35",</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>338</v>
+      </c>
+      <c r="H43">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>339</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="1"/>
+        <v>"36",</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>338</v>
+      </c>
+      <c r="H44">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>339</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="1"/>
+        <v>"37",</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>338</v>
+      </c>
+      <c r="H45">
+        <v>38</v>
+      </c>
+      <c r="I45" t="s">
+        <v>339</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="1"/>
+        <v>"38",</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>338</v>
+      </c>
+      <c r="H46">
+        <v>39</v>
+      </c>
+      <c r="I46" t="s">
+        <v>339</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="1"/>
+        <v>"39",</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>338</v>
+      </c>
+      <c r="H47">
+        <v>40</v>
+      </c>
+      <c r="I47" t="s">
+        <v>339</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" ref="J47:J58" si="2">G47&amp;H47&amp;I47</f>
+        <v>"40",</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>338</v>
+      </c>
+      <c r="H48">
+        <v>41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>339</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="2"/>
+        <v>"41",</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>338</v>
+      </c>
+      <c r="H49">
+        <v>42</v>
+      </c>
+      <c r="I49" t="s">
+        <v>339</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="2"/>
+        <v>"42",</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>338</v>
+      </c>
+      <c r="H50">
+        <v>43</v>
+      </c>
+      <c r="I50" t="s">
+        <v>339</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="2"/>
+        <v>"43",</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H51">
+        <v>44</v>
+      </c>
+      <c r="I51" t="s">
+        <v>339</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="2"/>
+        <v>"44",</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>338</v>
+      </c>
+      <c r="H52">
+        <v>45</v>
+      </c>
+      <c r="I52" t="s">
+        <v>339</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="2"/>
+        <v>"45",</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>338</v>
+      </c>
+      <c r="H53">
+        <v>46</v>
+      </c>
+      <c r="I53" t="s">
+        <v>339</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="2"/>
+        <v>"46",</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>338</v>
+      </c>
+      <c r="H54">
+        <v>47</v>
+      </c>
+      <c r="I54" t="s">
+        <v>339</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="2"/>
+        <v>"47",</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>338</v>
+      </c>
+      <c r="H55">
+        <v>48</v>
+      </c>
+      <c r="I55" t="s">
+        <v>339</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="2"/>
+        <v>"48",</v>
+      </c>
+    </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>338</v>
+      </c>
+      <c r="H56">
+        <v>49</v>
+      </c>
+      <c r="I56" t="s">
+        <v>339</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="2"/>
+        <v>"49",</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>338</v>
+      </c>
+      <c r="H57">
+        <v>50</v>
+      </c>
+      <c r="I57" t="s">
+        <v>339</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="2"/>
+        <v>"50",</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>338</v>
+      </c>
+      <c r="H58">
+        <v>51</v>
+      </c>
+      <c r="I58" t="s">
+        <v>339</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="2"/>
+        <v>"51",</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>338</v>
+      </c>
+      <c r="H59">
+        <v>52</v>
+      </c>
+      <c r="I59" t="s">
+        <v>339</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" ref="J59:J69" si="3">G59&amp;H59&amp;I59</f>
+        <v>"52",</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>338</v>
+      </c>
+      <c r="H60">
+        <v>53</v>
+      </c>
+      <c r="I60" t="s">
+        <v>339</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="3"/>
+        <v>"53",</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>338</v>
+      </c>
+      <c r="H61">
+        <v>54</v>
+      </c>
+      <c r="I61" t="s">
+        <v>339</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="3"/>
+        <v>"54",</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>338</v>
+      </c>
+      <c r="H62">
+        <v>55</v>
+      </c>
+      <c r="I62" t="s">
+        <v>339</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="3"/>
+        <v>"55",</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>338</v>
+      </c>
+      <c r="H63">
+        <v>56</v>
+      </c>
+      <c r="I63" t="s">
+        <v>339</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="3"/>
+        <v>"56",</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>338</v>
+      </c>
+      <c r="H64">
+        <v>57</v>
+      </c>
+      <c r="I64" t="s">
+        <v>339</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="3"/>
+        <v>"57",</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>338</v>
+      </c>
+      <c r="H65">
+        <v>58</v>
+      </c>
+      <c r="I65" t="s">
+        <v>339</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="3"/>
+        <v>"58",</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>338</v>
+      </c>
+      <c r="H66">
+        <v>59</v>
+      </c>
+      <c r="I66" t="s">
+        <v>339</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="3"/>
+        <v>"59",</v>
+      </c>
+    </row>
+    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>338</v>
+      </c>
+      <c r="H67">
+        <v>60</v>
+      </c>
+      <c r="I67" t="s">
+        <v>339</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="3"/>
+        <v>"60",</v>
+      </c>
+    </row>
+    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>338</v>
+      </c>
+      <c r="H68">
+        <v>61</v>
+      </c>
+      <c r="I68" t="s">
+        <v>339</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="3"/>
+        <v>"61",</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>338</v>
+      </c>
+      <c r="H69">
+        <v>62</v>
+      </c>
+      <c r="I69" t="s">
+        <v>339</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="3"/>
+        <v>"62",</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>338</v>
+      </c>
+      <c r="H70">
+        <v>63</v>
+      </c>
+      <c r="I70" t="s">
+        <v>339</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" ref="J70:J79" si="4">G70&amp;H70&amp;I70</f>
+        <v>"63",</v>
+      </c>
+    </row>
+    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>338</v>
+      </c>
+      <c r="H71">
+        <v>64</v>
+      </c>
+      <c r="I71" t="s">
+        <v>339</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="4"/>
+        <v>"64",</v>
+      </c>
+    </row>
+    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>338</v>
+      </c>
+      <c r="H72">
+        <v>65</v>
+      </c>
+      <c r="I72" t="s">
+        <v>339</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="4"/>
+        <v>"65",</v>
+      </c>
+    </row>
+    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>338</v>
+      </c>
+      <c r="H73">
+        <v>66</v>
+      </c>
+      <c r="I73" t="s">
+        <v>339</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="4"/>
+        <v>"66",</v>
+      </c>
+    </row>
+    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>338</v>
+      </c>
+      <c r="H74">
+        <v>67</v>
+      </c>
+      <c r="I74" t="s">
+        <v>339</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="4"/>
+        <v>"67",</v>
+      </c>
+    </row>
+    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>338</v>
+      </c>
+      <c r="H75">
+        <v>68</v>
+      </c>
+      <c r="I75" t="s">
+        <v>339</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="4"/>
+        <v>"68",</v>
+      </c>
+    </row>
+    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>338</v>
+      </c>
+      <c r="H76">
+        <v>69</v>
+      </c>
+      <c r="I76" t="s">
+        <v>339</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="4"/>
+        <v>"69",</v>
+      </c>
+    </row>
+    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>338</v>
+      </c>
+      <c r="H77">
+        <v>70</v>
+      </c>
+      <c r="I77" t="s">
+        <v>339</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="4"/>
+        <v>"70",</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>338</v>
+      </c>
+      <c r="H78">
+        <v>71</v>
+      </c>
+      <c r="I78" t="s">
+        <v>339</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="4"/>
+        <v>"71",</v>
+      </c>
+    </row>
+    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>338</v>
+      </c>
+      <c r="H79">
+        <v>72</v>
+      </c>
+      <c r="I79" t="s">
+        <v>339</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="4"/>
+        <v>"72",</v>
+      </c>
+    </row>
+    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>338</v>
+      </c>
+      <c r="H80">
+        <v>73</v>
+      </c>
+      <c r="I80" t="s">
+        <v>339</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" ref="J80:J89" si="5">G80&amp;H80&amp;I80</f>
+        <v>"73",</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>338</v>
+      </c>
+      <c r="H81">
+        <v>74</v>
+      </c>
+      <c r="I81" t="s">
+        <v>339</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="5"/>
+        <v>"74",</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>338</v>
+      </c>
+      <c r="H82">
+        <v>75</v>
+      </c>
+      <c r="I82" t="s">
+        <v>339</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="5"/>
+        <v>"75",</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>338</v>
+      </c>
+      <c r="H83">
+        <v>76</v>
+      </c>
+      <c r="I83" t="s">
+        <v>339</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="5"/>
+        <v>"76",</v>
+      </c>
+    </row>
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>338</v>
+      </c>
+      <c r="H84">
+        <v>77</v>
+      </c>
+      <c r="I84" t="s">
+        <v>339</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="5"/>
+        <v>"77",</v>
+      </c>
+    </row>
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>338</v>
+      </c>
+      <c r="H85">
+        <v>78</v>
+      </c>
+      <c r="I85" t="s">
+        <v>339</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="5"/>
+        <v>"78",</v>
+      </c>
+    </row>
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>338</v>
+      </c>
+      <c r="H86">
+        <v>79</v>
+      </c>
+      <c r="I86" t="s">
+        <v>339</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="5"/>
+        <v>"79",</v>
+      </c>
+    </row>
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>338</v>
+      </c>
+      <c r="H87">
+        <v>80</v>
+      </c>
+      <c r="I87" t="s">
+        <v>339</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="5"/>
+        <v>"80",</v>
+      </c>
+    </row>
+    <row r="88" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>338</v>
+      </c>
+      <c r="H88">
+        <v>81</v>
+      </c>
+      <c r="I88" t="s">
+        <v>339</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="5"/>
+        <v>"81",</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4A9989-40F3-40D3-8B94-7874F8B238D1}">
+  <dimension ref="G7:K88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="139.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f>J8&amp;J9&amp;J10&amp;J11&amp;J12&amp;J13&amp;J14&amp;J15&amp;J16&amp;J17&amp;J18&amp;J19&amp;J20&amp;J21&amp;J22&amp;J23&amp;J24&amp;J25&amp;J26&amp;J27&amp;J28&amp;J29&amp;J30&amp;J31&amp;J32&amp;J33&amp;J34&amp;J35&amp;J36&amp;J37&amp;J38&amp;J39&amp;J40&amp;J41&amp;J42&amp;J43&amp;J44&amp;J45&amp;J46&amp;J47&amp;J48&amp;J49&amp;J50&amp;J51&amp;J52&amp;J53&amp;J54&amp;J55&amp;J56&amp;J57&amp;J58&amp;J59&amp;J60&amp;J61&amp;J62&amp;J63&amp;J64&amp;J65&amp;J66&amp;J67&amp;J68&amp;J69&amp;J70&amp;J71&amp;J72&amp;J73&amp;J74&amp;J75&amp;J76&amp;J77&amp;J78&amp;J79&amp;J80&amp;J81&amp;J82&amp;J83&amp;J84&amp;J85&amp;J86&amp;J87&amp;J88</f>
+        <v>{"1","2","3","4","5","6","7","8","9","10","11","12","13","14","15","16","17","18","19","20","21","22","23","24","25","26","27","28","29","30","31","32","33","34","35","36","37","38","39","40","41","42","43","44","45","46","47","48","49","50","51","52","53","54","55","56","57","58","59","60","61","62","63","64","65","66","67","68","69","70","71","72","73","74","75","76","77","78","79","80","81"}</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>341</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>339</v>
+      </c>
+      <c r="J8" t="str">
+        <f>G8&amp;H8&amp;I8</f>
+        <v>{"1",</v>
+      </c>
+    </row>
+    <row r="9" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>339</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9:J72" si="0">G9&amp;H9&amp;I9</f>
+        <v>"2",</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>338</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>339</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>"3",</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>338</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>339</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>"4",</v>
+      </c>
+    </row>
+    <row r="12" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>339</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>"5",</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>338</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>339</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>"6",</v>
+      </c>
+    </row>
+    <row r="14" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>338</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>339</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>"7",</v>
+      </c>
+    </row>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>338</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>339</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>"8",</v>
+      </c>
+    </row>
+    <row r="16" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>339</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>"9",</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>338</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>339</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>"10",</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>338</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>339</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>"11",</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>338</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
+        <v>339</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>"12",</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>338</v>
+      </c>
+      <c r="H20">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>339</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>"13",</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>338</v>
+      </c>
+      <c r="H21">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>339</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>"14",</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>338</v>
+      </c>
+      <c r="H22">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>339</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>"15",</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>339</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>"16",</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>338</v>
+      </c>
+      <c r="H24">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>339</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>"17",</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>338</v>
+      </c>
+      <c r="H25">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>339</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>"18",</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>338</v>
+      </c>
+      <c r="H26">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>339</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>"19",</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>338</v>
+      </c>
+      <c r="H27">
+        <v>20</v>
+      </c>
+      <c r="I27" t="s">
+        <v>339</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>"20",</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>338</v>
+      </c>
+      <c r="H28">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>339</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>"21",</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>338</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29" t="s">
+        <v>339</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>"22",</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>338</v>
+      </c>
+      <c r="H30">
+        <v>23</v>
+      </c>
+      <c r="I30" t="s">
+        <v>339</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>"23",</v>
+      </c>
+    </row>
+    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>338</v>
+      </c>
+      <c r="H31">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>339</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>"24",</v>
+      </c>
+    </row>
+    <row r="32" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>338</v>
+      </c>
+      <c r="H32">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>339</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>"25",</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>338</v>
+      </c>
+      <c r="H33">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
+        <v>339</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>"26",</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>338</v>
+      </c>
+      <c r="H34">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
+        <v>339</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>"27",</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>338</v>
+      </c>
+      <c r="H35">
+        <v>28</v>
+      </c>
+      <c r="I35" t="s">
+        <v>339</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>"28",</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>338</v>
+      </c>
+      <c r="H36">
+        <v>29</v>
+      </c>
+      <c r="I36" t="s">
+        <v>339</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>"29",</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>338</v>
+      </c>
+      <c r="H37">
+        <v>30</v>
+      </c>
+      <c r="I37" t="s">
+        <v>339</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>"30",</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>338</v>
+      </c>
+      <c r="H38">
+        <v>31</v>
+      </c>
+      <c r="I38" t="s">
+        <v>339</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>"31",</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>338</v>
+      </c>
+      <c r="H39">
+        <v>32</v>
+      </c>
+      <c r="I39" t="s">
+        <v>339</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>"32",</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>338</v>
+      </c>
+      <c r="H40">
+        <v>33</v>
+      </c>
+      <c r="I40" t="s">
+        <v>339</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>"33",</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>338</v>
+      </c>
+      <c r="H41">
+        <v>34</v>
+      </c>
+      <c r="I41" t="s">
+        <v>339</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>"34",</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>338</v>
+      </c>
+      <c r="H42">
+        <v>35</v>
+      </c>
+      <c r="I42" t="s">
+        <v>339</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>"35",</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>338</v>
+      </c>
+      <c r="H43">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>339</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v>"36",</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>338</v>
+      </c>
+      <c r="H44">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>339</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>"37",</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>338</v>
+      </c>
+      <c r="H45">
+        <v>38</v>
+      </c>
+      <c r="I45" t="s">
+        <v>339</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v>"38",</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>338</v>
+      </c>
+      <c r="H46">
+        <v>39</v>
+      </c>
+      <c r="I46" t="s">
+        <v>339</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="0"/>
+        <v>"39",</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>338</v>
+      </c>
+      <c r="H47">
+        <v>40</v>
+      </c>
+      <c r="I47" t="s">
+        <v>339</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="0"/>
+        <v>"40",</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>338</v>
+      </c>
+      <c r="H48">
+        <v>41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>339</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="0"/>
+        <v>"41",</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>338</v>
+      </c>
+      <c r="H49">
+        <v>42</v>
+      </c>
+      <c r="I49" t="s">
+        <v>339</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="0"/>
+        <v>"42",</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>338</v>
+      </c>
+      <c r="H50">
+        <v>43</v>
+      </c>
+      <c r="I50" t="s">
+        <v>339</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="0"/>
+        <v>"43",</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>338</v>
+      </c>
+      <c r="H51">
+        <v>44</v>
+      </c>
+      <c r="I51" t="s">
+        <v>339</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="0"/>
+        <v>"44",</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>338</v>
+      </c>
+      <c r="H52">
+        <v>45</v>
+      </c>
+      <c r="I52" t="s">
+        <v>339</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="0"/>
+        <v>"45",</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>338</v>
+      </c>
+      <c r="H53">
+        <v>46</v>
+      </c>
+      <c r="I53" t="s">
+        <v>339</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="0"/>
+        <v>"46",</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>338</v>
+      </c>
+      <c r="H54">
+        <v>47</v>
+      </c>
+      <c r="I54" t="s">
+        <v>339</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="0"/>
+        <v>"47",</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>338</v>
+      </c>
+      <c r="H55">
+        <v>48</v>
+      </c>
+      <c r="I55" t="s">
+        <v>339</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="0"/>
+        <v>"48",</v>
+      </c>
+    </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>338</v>
+      </c>
+      <c r="H56">
+        <v>49</v>
+      </c>
+      <c r="I56" t="s">
+        <v>339</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="0"/>
+        <v>"49",</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>338</v>
+      </c>
+      <c r="H57">
+        <v>50</v>
+      </c>
+      <c r="I57" t="s">
+        <v>339</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="0"/>
+        <v>"50",</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>338</v>
+      </c>
+      <c r="H58">
+        <v>51</v>
+      </c>
+      <c r="I58" t="s">
+        <v>339</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="0"/>
+        <v>"51",</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>338</v>
+      </c>
+      <c r="H59">
+        <v>52</v>
+      </c>
+      <c r="I59" t="s">
+        <v>339</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="0"/>
+        <v>"52",</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>338</v>
+      </c>
+      <c r="H60">
+        <v>53</v>
+      </c>
+      <c r="I60" t="s">
+        <v>339</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="0"/>
+        <v>"53",</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>338</v>
+      </c>
+      <c r="H61">
+        <v>54</v>
+      </c>
+      <c r="I61" t="s">
+        <v>339</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="0"/>
+        <v>"54",</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>338</v>
+      </c>
+      <c r="H62">
+        <v>55</v>
+      </c>
+      <c r="I62" t="s">
+        <v>339</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="0"/>
+        <v>"55",</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>338</v>
+      </c>
+      <c r="H63">
+        <v>56</v>
+      </c>
+      <c r="I63" t="s">
+        <v>339</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="0"/>
+        <v>"56",</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>338</v>
+      </c>
+      <c r="H64">
+        <v>57</v>
+      </c>
+      <c r="I64" t="s">
+        <v>339</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="0"/>
+        <v>"57",</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>338</v>
+      </c>
+      <c r="H65">
+        <v>58</v>
+      </c>
+      <c r="I65" t="s">
+        <v>339</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="0"/>
+        <v>"58",</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>338</v>
+      </c>
+      <c r="H66">
+        <v>59</v>
+      </c>
+      <c r="I66" t="s">
+        <v>339</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="0"/>
+        <v>"59",</v>
+      </c>
+    </row>
+    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>338</v>
+      </c>
+      <c r="H67">
+        <v>60</v>
+      </c>
+      <c r="I67" t="s">
+        <v>339</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="0"/>
+        <v>"60",</v>
+      </c>
+    </row>
+    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>338</v>
+      </c>
+      <c r="H68">
+        <v>61</v>
+      </c>
+      <c r="I68" t="s">
+        <v>339</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="0"/>
+        <v>"61",</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>338</v>
+      </c>
+      <c r="H69">
+        <v>62</v>
+      </c>
+      <c r="I69" t="s">
+        <v>339</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="0"/>
+        <v>"62",</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>338</v>
+      </c>
+      <c r="H70">
+        <v>63</v>
+      </c>
+      <c r="I70" t="s">
+        <v>339</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="0"/>
+        <v>"63",</v>
+      </c>
+    </row>
+    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>338</v>
+      </c>
+      <c r="H71">
+        <v>64</v>
+      </c>
+      <c r="I71" t="s">
+        <v>339</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="0"/>
+        <v>"64",</v>
+      </c>
+    </row>
+    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>338</v>
+      </c>
+      <c r="H72">
+        <v>65</v>
+      </c>
+      <c r="I72" t="s">
+        <v>339</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="0"/>
+        <v>"65",</v>
+      </c>
+    </row>
+    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>338</v>
+      </c>
+      <c r="H73">
+        <v>66</v>
+      </c>
+      <c r="I73" t="s">
+        <v>339</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" ref="J73:J88" si="1">G73&amp;H73&amp;I73</f>
+        <v>"66",</v>
+      </c>
+    </row>
+    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>338</v>
+      </c>
+      <c r="H74">
+        <v>67</v>
+      </c>
+      <c r="I74" t="s">
+        <v>339</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="1"/>
+        <v>"67",</v>
+      </c>
+    </row>
+    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>338</v>
+      </c>
+      <c r="H75">
+        <v>68</v>
+      </c>
+      <c r="I75" t="s">
+        <v>339</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="1"/>
+        <v>"68",</v>
+      </c>
+    </row>
+    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>338</v>
+      </c>
+      <c r="H76">
+        <v>69</v>
+      </c>
+      <c r="I76" t="s">
+        <v>339</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="1"/>
+        <v>"69",</v>
+      </c>
+    </row>
+    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>338</v>
+      </c>
+      <c r="H77">
+        <v>70</v>
+      </c>
+      <c r="I77" t="s">
+        <v>339</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="1"/>
+        <v>"70",</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>338</v>
+      </c>
+      <c r="H78">
+        <v>71</v>
+      </c>
+      <c r="I78" t="s">
+        <v>339</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="1"/>
+        <v>"71",</v>
+      </c>
+    </row>
+    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>338</v>
+      </c>
+      <c r="H79">
+        <v>72</v>
+      </c>
+      <c r="I79" t="s">
+        <v>339</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="1"/>
+        <v>"72",</v>
+      </c>
+    </row>
+    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>338</v>
+      </c>
+      <c r="H80">
+        <v>73</v>
+      </c>
+      <c r="I80" t="s">
+        <v>339</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="1"/>
+        <v>"73",</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>338</v>
+      </c>
+      <c r="H81">
+        <v>74</v>
+      </c>
+      <c r="I81" t="s">
+        <v>339</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="1"/>
+        <v>"74",</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>338</v>
+      </c>
+      <c r="H82">
+        <v>75</v>
+      </c>
+      <c r="I82" t="s">
+        <v>339</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="1"/>
+        <v>"75",</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>338</v>
+      </c>
+      <c r="H83">
+        <v>76</v>
+      </c>
+      <c r="I83" t="s">
+        <v>339</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="1"/>
+        <v>"76",</v>
+      </c>
+    </row>
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>338</v>
+      </c>
+      <c r="H84">
+        <v>77</v>
+      </c>
+      <c r="I84" t="s">
+        <v>339</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="1"/>
+        <v>"77",</v>
+      </c>
+    </row>
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>338</v>
+      </c>
+      <c r="H85">
+        <v>78</v>
+      </c>
+      <c r="I85" t="s">
+        <v>339</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="1"/>
+        <v>"78",</v>
+      </c>
+    </row>
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>338</v>
+      </c>
+      <c r="H86">
+        <v>79</v>
+      </c>
+      <c r="I86" t="s">
+        <v>339</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="1"/>
+        <v>"79",</v>
+      </c>
+    </row>
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>338</v>
+      </c>
+      <c r="H87">
+        <v>80</v>
+      </c>
+      <c r="I87" t="s">
+        <v>339</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="1"/>
+        <v>"80",</v>
+      </c>
+    </row>
+    <row r="88" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>338</v>
+      </c>
+      <c r="H88">
+        <v>81</v>
+      </c>
+      <c r="I88" t="s">
+        <v>340</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="1"/>
+        <v>"81"}</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add tests for duplicates in row and column
</commit_message>
<xml_diff>
--- a/Sudoku_Grid.xlsx
+++ b/Sudoku_Grid.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\soe-mobile-sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91056B73-70F4-46F9-AB60-F877D0592402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B402E0F-53A3-4600-ACB9-A1E3ACAB410B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{8CBA904F-269B-4B80-8211-F0CFD0911C38}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{8CBA904F-269B-4B80-8211-F0CFD0911C38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet6 (2)" sheetId="7" r:id="rId7"/>
+    <sheet name="ARRAY_GRID" sheetId="8" r:id="rId1"/>
+    <sheet name="GUI_GRID" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet6 (2)" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="344">
   <si>
     <t xml:space="preserve"> Field01 = sudokuStringArray[0];</t>
   </si>
@@ -1066,13 +1067,19 @@
   </si>
   <si>
     <t>{"</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,6 +1097,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1250,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1285,6 +1299,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1598,11 +1618,463 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCB45F4-002F-485F-8A0B-0CA335DE9DA0}">
+  <dimension ref="B5:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="5" style="10" customWidth="1"/>
+    <col min="5" max="12" width="5" customWidth="1"/>
+    <col min="13" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="2:12" s="10" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>3</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4</v>
+      </c>
+      <c r="H6" s="10">
+        <v>5</v>
+      </c>
+      <c r="I6" s="10">
+        <v>6</v>
+      </c>
+      <c r="J6" s="10">
+        <v>7</v>
+      </c>
+      <c r="K6" s="10">
+        <v>8</v>
+      </c>
+      <c r="L6" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="10">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D7+9</f>
+        <v>9</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:L15" si="0">E7+9</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15"/>
+      <c r="C9" s="10">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" ref="D9:D15" si="1">D8+9</f>
+        <v>18</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K9" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="L9" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D9+9</f>
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <f>E9+9</f>
+        <v>28</v>
+      </c>
+      <c r="F10" s="3">
+        <f>F9+9</f>
+        <v>29</v>
+      </c>
+      <c r="G10" s="1">
+        <f>G9+9</f>
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <f>H9+9</f>
+        <v>31</v>
+      </c>
+      <c r="I10" s="3">
+        <f>I9+9</f>
+        <v>32</v>
+      </c>
+      <c r="J10" s="1">
+        <f>J9+9</f>
+        <v>33</v>
+      </c>
+      <c r="K10" s="2">
+        <f>K9+9</f>
+        <v>34</v>
+      </c>
+      <c r="L10" s="3">
+        <f>L9+9</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="10">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="K12" s="8">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="L12" s="9">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="10">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <f>D12+9</f>
+        <v>54</v>
+      </c>
+      <c r="E13" s="2">
+        <f>E12+9</f>
+        <v>55</v>
+      </c>
+      <c r="F13" s="3">
+        <f>F12+9</f>
+        <v>56</v>
+      </c>
+      <c r="G13" s="1">
+        <f>G12+9</f>
+        <v>57</v>
+      </c>
+      <c r="H13" s="2">
+        <f>H12+9</f>
+        <v>58</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I12+9</f>
+        <v>59</v>
+      </c>
+      <c r="J13" s="1">
+        <f>J12+9</f>
+        <v>60</v>
+      </c>
+      <c r="K13" s="2">
+        <f>K12+9</f>
+        <v>61</v>
+      </c>
+      <c r="L13" s="3">
+        <f>L12+9</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="10">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15"/>
+      <c r="C15" s="10">
+        <v>9</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="K15" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="L15" s="9">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="3:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="3:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="3:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="D5:L5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285140B6-F8BD-4404-8803-428FED8FB827}">
   <dimension ref="C6:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="N8" activeCellId="2" sqref="E8 J8 N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E0D1B1-5B98-4861-B153-A9DD139C652E}">
   <dimension ref="C5:H224"/>
   <sheetViews>
@@ -4454,7 +4926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F607C08-F6DC-4A76-8ADE-42A6E93DE759}">
   <dimension ref="D4:J262"/>
   <sheetViews>
@@ -6712,7 +7184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B86DC8-5D40-4BCA-9E3F-1E25F0AC9493}">
   <dimension ref="C5:I141"/>
   <sheetViews>
@@ -8417,7 +8889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE7FA67-3B85-4D66-8F07-D6BFFD057CF0}">
   <dimension ref="C3:H111"/>
   <sheetViews>
@@ -10006,7 +10478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96F4CB0-1FB2-4D82-ACB0-0C881D5B76C8}">
   <dimension ref="G7:K88"/>
   <sheetViews>
@@ -11116,7 +11588,7 @@
         <v>339</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" ref="J80:J89" si="5">G80&amp;H80&amp;I80</f>
+        <f t="shared" ref="J80:J88" si="5">G80&amp;H80&amp;I80</f>
         <v>"73",</v>
       </c>
     </row>
@@ -11246,11 +11718,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4A9989-40F3-40D3-8B94-7874F8B238D1}">
   <dimension ref="G7:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>